<commit_message>
Update to version 6.0.0 of cht-conf
</commit_message>
<xml_diff>
--- a/basic-forms/forms/training/ui_change_floating_action_button.xlsx
+++ b/basic-forms/forms/training/ui_change_floating_action_button.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId3"/>
@@ -144,9 +144,8 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">The unique ID that identifies this form to tools that use it. It may not contain spaces and must start with a letter or underscore. You should use a short, descriptive name and can use underscores to separate words. 
-For example: bench_inventory_2021
-You can change the form_title as much as you would like but if you change the form_id, it will be considered a different form definition.</t>
+          <t xml:space="preserve">The unique version code that identifies the current state of the form. A common convention is to use a format like yyyymmddrr. For example, 2017021501 is the 1st revision from Feb 15th, 2017.
+By default, this template uses a formula to create a date-based version that will update automatically.</t>
         </r>
       </text>
     </comment>
@@ -158,24 +157,11 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">The unique version code that identifies the current state of the form. A common convention is to use a format like yyyymmddrr. For example, 2017021501 is the 1st revision from Feb 15th, 2017.
-By default, this template uses a formula to create a date-based version that will update automatically.</t>
+          <t xml:space="preserve">Set to ‘pages’ to indicate that groups with the `field-list` appearance represent separate form pages (and all other questions will be shown on their own page). </t>
         </r>
       </text>
     </comment>
     <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Set to ‘pages’ to indicate that groups with the `field-list` appearance represent separate form pages (and all other questions will be shown on their own page). </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -192,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -290,9 +276,6 @@
     <t xml:space="preserve">form_title</t>
   </si>
   <si>
-    <t xml:space="preserve">form_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">version</t>
   </si>
   <si>
@@ -303,9 +286,6 @@
   </si>
   <si>
     <t xml:space="preserve">Floating action button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">training:new_ui_change_floating_action_button</t>
   </si>
   <si>
     <t xml:space="preserve">pages</t>
@@ -792,7 +772,7 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
@@ -1014,7 +994,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A28:F10000 A27:B27 D2:F27 A2:C26 C27">
+  <conditionalFormatting sqref="A2:F10000">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$A2="begin_group"</formula>
     </cfRule>
@@ -1036,7 +1016,7 @@
       <formula>AND(ISBLANK(B2), NOT(ISBLANK($A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C10000 C2:C26 C27">
+  <conditionalFormatting sqref="C2:C10000">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND(ISBLANK(C2),NOT(OR(ISBLANK($A2),$A2="calculate")))</formula>
     </cfRule>
@@ -1067,18 +1047,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="17.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="16.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="32.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="32.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1094,26 +1073,20 @@
       <c r="D1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="str">
+        <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
+        <v>20260114090126</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C2" s="6" t="str">
-        <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20251119134144</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>